<commit_message>
record 14 e documentazione
</commit_message>
<xml_diff>
--- a/input_complex_data.xlsx
+++ b/input_complex_data.xlsx
@@ -3515,9 +3515,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YYYY"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3539,87 +3539,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -3656,77 +3575,20 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -3745,7 +3607,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3769,54 +3631,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3827,7 +3641,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3835,65 +3649,49 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -3905,7 +3703,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -3921,7 +3719,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -11652,8 +11450,8 @@
   </sheetPr>
   <dimension ref="A1:M962"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12219,7 +12017,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>13</v>
       </c>

</xml_diff>